<commit_message>
UP Actualización de archivos
</commit_message>
<xml_diff>
--- a/Data/OriginalData/Agencia2017/libro_códigos.xlsx
+++ b/Data/OriginalData/Agencia2017/libro_códigos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josedanielconejeros/Dropbox/Fondecyt 2019-2021(AsistenteJC)/socializacion_politica_adolescentes/Data/OriginalData/Agencia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josedanielconejeros/Dropbox/Fondecyt 2019-2021(AsistenteJC)/socializacion_politica_adolescentes/Data/OriginalData/Agencia2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5319A63A-A796-7A42-B1C9-042462445B54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668645CF-1C02-2245-9B06-5AA5C2F7E051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" xr2:uid="{66D1939E-F540-4C41-9398-9710D77FB3D3}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{66D1939E-F540-4C41-9398-9710D77FB3D3}"/>
   </bookViews>
   <sheets>
     <sheet name="completo" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6040" uniqueCount="1368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6040" uniqueCount="1369">
   <si>
     <t>idAlumno</t>
   </si>
@@ -4145,6 +4145,9 @@
   </si>
   <si>
     <t>Postgrado, Magister, Doctorado</t>
+  </si>
+  <si>
+    <t>Autoeficacia Ciudadana</t>
   </si>
 </sst>
 </file>
@@ -4515,8 +4518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8A2E0A-F877-974D-8C0E-9CC503976022}">
   <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9653,8 +9656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4145EC5A-2CEF-EB47-8CDF-8C2465EE6ED9}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E230" sqref="E230"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11817,7 +11820,7 @@
         <v>693</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>236</v>
+        <v>1368</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>237</v>
@@ -11841,7 +11844,7 @@
         <v>693</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>236</v>
+        <v>1368</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>240</v>
@@ -11865,7 +11868,7 @@
         <v>693</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>236</v>
+        <v>1368</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>242</v>
@@ -11889,7 +11892,7 @@
         <v>693</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>236</v>
+        <v>1368</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>244</v>
@@ -11913,7 +11916,7 @@
         <v>693</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>236</v>
+        <v>1368</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>246</v>
@@ -11937,7 +11940,7 @@
         <v>693</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>236</v>
+        <v>1368</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>248</v>
@@ -11961,7 +11964,7 @@
         <v>693</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>236</v>
+        <v>1368</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>250</v>
@@ -21464,8 +21467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFC846A-09B5-4C45-AF4B-7F6BDCC6C70A}">
   <dimension ref="A1:J225"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23008,10 +23011,10 @@
       <c r="B88" t="s">
         <v>683</v>
       </c>
-      <c r="C88" t="s">
-        <v>236</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="C88" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>237</v>
       </c>
       <c r="E88" t="s">
@@ -23031,10 +23034,10 @@
       <c r="B89" t="s">
         <v>683</v>
       </c>
-      <c r="C89" t="s">
-        <v>236</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C89" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>240</v>
       </c>
       <c r="E89" t="s">
@@ -23051,10 +23054,10 @@
       <c r="B90" t="s">
         <v>683</v>
       </c>
-      <c r="C90" t="s">
-        <v>236</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="C90" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>242</v>
       </c>
       <c r="E90" t="s">
@@ -23071,10 +23074,10 @@
       <c r="B91" t="s">
         <v>683</v>
       </c>
-      <c r="C91" t="s">
-        <v>236</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="C91" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>244</v>
       </c>
       <c r="E91" t="s">
@@ -23091,10 +23094,10 @@
       <c r="B92" t="s">
         <v>683</v>
       </c>
-      <c r="C92" t="s">
-        <v>236</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="C92" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>246</v>
       </c>
       <c r="E92" t="s">
@@ -23111,10 +23114,10 @@
       <c r="B93" t="s">
         <v>683</v>
       </c>
-      <c r="C93" t="s">
-        <v>236</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="C93" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>248</v>
       </c>
       <c r="E93" t="s">
@@ -23131,10 +23134,10 @@
       <c r="B94" t="s">
         <v>683</v>
       </c>
-      <c r="C94" t="s">
-        <v>236</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="C94" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>250</v>
       </c>
       <c r="E94" t="s">

</xml_diff>

<commit_message>
UP Codificación de variables
</commit_message>
<xml_diff>
--- a/Data/OriginalData/Agencia2017/libro_códigos.xlsx
+++ b/Data/OriginalData/Agencia2017/libro_códigos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josedanielconejeros/Dropbox/Fondecyt 2019-2021(AsistenteJC)/socializacion_politica_adolescentes/Data/OriginalData/Agencia2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668645CF-1C02-2245-9B06-5AA5C2F7E051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1E470D-F1B9-AC4B-9A5B-372EDE5CDD7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{66D1939E-F540-4C41-9398-9710D77FB3D3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="6" xr2:uid="{66D1939E-F540-4C41-9398-9710D77FB3D3}"/>
   </bookViews>
   <sheets>
     <sheet name="completo" sheetId="9" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Etiquetas" sheetId="8" r:id="rId4"/>
     <sheet name="Padres" sheetId="4" r:id="rId5"/>
     <sheet name="Alumnos" sheetId="5" r:id="rId6"/>
+    <sheet name="Escalas" sheetId="10" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">alumnos_padres!$A$1:$I$257</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6040" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6273" uniqueCount="1374">
   <si>
     <t>idAlumno</t>
   </si>
@@ -4148,13 +4149,28 @@
   </si>
   <si>
     <t>Autoeficacia Ciudadana</t>
+  </si>
+  <si>
+    <t>Tema</t>
+  </si>
+  <si>
+    <t>Pregunta</t>
+  </si>
+  <si>
+    <t>Atributos</t>
+  </si>
+  <si>
+    <t>cuest_alum</t>
+  </si>
+  <si>
+    <t>cuest_pad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4177,13 +4193,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4198,10 +4244,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9656,8 +9707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4145EC5A-2CEF-EB47-8CDF-8C2465EE6ED9}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G46" activeCellId="3" sqref="B46:B55 D46:D55 F46:F55 G46:H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21467,8 +21518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFC846A-09B5-4C45-AF4B-7F6BDCC6C70A}">
   <dimension ref="A1:J225"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25443,4 +25494,821 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAE948D-DDE8-CF4D-A8F9-6A9A061A82A3}">
+  <dimension ref="A1:E48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="25.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="69.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>